<commit_message>
41316 Laptop -- Final analysis done
</commit_message>
<xml_diff>
--- a/Normalization/SummaryDataCV.xlsx
+++ b/Normalization/SummaryDataCV.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32120" yWindow="540" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="-22900" yWindow="0" windowWidth="25600" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryDataCV.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,33 +33,6 @@
     <t>&lt;= 30</t>
   </si>
   <si>
-    <t>150 (25%)</t>
-  </si>
-  <si>
-    <t>318 (54%)</t>
-  </si>
-  <si>
-    <t>434 (74%)</t>
-  </si>
-  <si>
-    <t>92 (23%)</t>
-  </si>
-  <si>
-    <t>211 (54%)</t>
-  </si>
-  <si>
-    <t>297 (76%)</t>
-  </si>
-  <si>
-    <t>269 (33%)</t>
-  </si>
-  <si>
-    <t>481 (59%)</t>
-  </si>
-  <si>
-    <t>608 (75%)</t>
-  </si>
-  <si>
     <t>63 (12%)</t>
   </si>
   <si>
@@ -69,24 +42,6 @@
     <t>348 (64%)</t>
   </si>
   <si>
-    <t>125 (20%)</t>
-  </si>
-  <si>
-    <t>272 (44%)</t>
-  </si>
-  <si>
-    <t>427 (70%)</t>
-  </si>
-  <si>
-    <t>54 (15%)</t>
-  </si>
-  <si>
-    <t>166 (46%)</t>
-  </si>
-  <si>
-    <t>263 (73%)</t>
-  </si>
-  <si>
     <t>SCN_Pos</t>
   </si>
   <si>
@@ -109,6 +64,51 @@
   </si>
   <si>
     <t>Combined</t>
+  </si>
+  <si>
+    <t>145 (25%)</t>
+  </si>
+  <si>
+    <t>311 (54%)</t>
+  </si>
+  <si>
+    <t>424 (73%)</t>
+  </si>
+  <si>
+    <t>89 (23%)</t>
+  </si>
+  <si>
+    <t>208 (54%)</t>
+  </si>
+  <si>
+    <t>293 (76%)</t>
+  </si>
+  <si>
+    <t>263 (33%)</t>
+  </si>
+  <si>
+    <t>473 (59%)</t>
+  </si>
+  <si>
+    <t>599 (75%)</t>
+  </si>
+  <si>
+    <t>121 (20%)</t>
+  </si>
+  <si>
+    <t>263 (44%)</t>
+  </si>
+  <si>
+    <t>418 (69%)</t>
+  </si>
+  <si>
+    <t>52(15%)</t>
+  </si>
+  <si>
+    <t>162 (46%)</t>
+  </si>
+  <si>
+    <t>259 (73%)</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -634,22 +634,22 @@
     <row r="1" spans="1:7" ht="20">
       <c r="A1" s="3"/>
       <c r="B1" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40">
@@ -657,22 +657,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="7">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="C2" s="8">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D2" s="7">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="E2" s="8">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="F2" s="7">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="G2" s="8">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20">
@@ -680,22 +680,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20">
@@ -703,22 +703,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20">
@@ -726,64 +726,64 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="C6" s="8">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D6" s="7">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="E6" s="8">
         <v>348</v>
       </c>
       <c r="F6" s="7">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="G6" s="8">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B7" s="9">
         <f>SUM(B6:C6)</f>
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="9">
         <f>SUM(D6:E6)</f>
-        <v>956</v>
+        <v>947</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="9">
         <f>SUM(F6:G6)</f>
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="G7" s="10"/>
     </row>

</xml_diff>